<commit_message>
feat: Add Excel export functionality when adding new wine
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data.xlsx
+++ b/backend/src/main/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\Projets\Stock V3\backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840C13D3-1988-4F32-AF4A-8FC806B579A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEE7551-CF85-405A-ADA4-0DFC938AD2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{866AF031-A8F6-4310-B6CB-F8A451908F4D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Domaine</t>
   </si>
@@ -62,7 +62,25 @@
     <t>Geanthet Pansiot</t>
   </si>
   <si>
-    <t>Gevrey-Chambertin "Vieilles Vignes"</t>
+    <t>Appellation</t>
+  </si>
+  <si>
+    <t>Chablis</t>
+  </si>
+  <si>
+    <t>Gevrey-Chambertin</t>
+  </si>
+  <si>
+    <t>"Vieilles Vignes"</t>
+  </si>
+  <si>
+    <t>ze</t>
+  </si>
+  <si>
+    <t>ze2</t>
+  </si>
+  <si>
+    <t>ze3</t>
   </si>
 </sst>
 </file>
@@ -448,20 +466,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D315F42-56D0-4B9B-B00B-79278325E538}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="2" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -472,44 +490,73 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>160</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="F3">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>90</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2018</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>28</v>
+      </c>
+      <c r="F4">
         <v>7</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ExcelService and Wine model to ensure data integrity, add logging and new values
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data.xlsx
+++ b/backend/src/main/resources/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\Projets\Stock V3\backend\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\Projets\Stock-V3\backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEE7551-CF85-405A-ADA4-0DFC938AD2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4928BCD8-447F-4985-81BF-04D2BAF2F14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{866AF031-A8F6-4310-B6CB-F8A451908F4D}"/>
   </bookViews>
@@ -36,23 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Domaine</t>
   </si>
   <si>
-    <t>Cuvée</t>
-  </si>
-  <si>
-    <t>Quantité</t>
-  </si>
-  <si>
-    <t>Prix</t>
-  </si>
-  <si>
-    <t>Millésime</t>
-  </si>
-  <si>
     <t>Terroir Chapelle</t>
   </si>
   <si>
@@ -74,13 +62,61 @@
     <t>"Vieilles Vignes"</t>
   </si>
   <si>
-    <t>ze</t>
-  </si>
-  <si>
-    <t>ze2</t>
-  </si>
-  <si>
-    <t>ze3</t>
+    <t>Brut Vintage - Magnum</t>
+  </si>
+  <si>
+    <t>Dom Pérignon</t>
+  </si>
+  <si>
+    <t>Brut Vintage Rosé</t>
+  </si>
+  <si>
+    <t>Champagne</t>
+  </si>
+  <si>
+    <t>Bourgogne</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Cave Royale</t>
+  </si>
+  <si>
+    <t>Cavesa</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Pricetobuy</t>
+  </si>
+  <si>
+    <t>Pricetosell</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Millesime</t>
+  </si>
+  <si>
+    <t>Cuvee</t>
+  </si>
+  <si>
+    <t>Region</t>
   </si>
 </sst>
 </file>
@@ -124,12 +160,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -466,97 +511,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D315F42-56D0-4B9B-B00B-79278325E538}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="2" max="3" width="32.5703125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="19.85546875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="10.140625" style="4" customWidth="1"/>
+    <col min="10" max="12" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>2</v>
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>160</v>
-      </c>
-      <c r="F2">
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1">
+        <v>138</v>
+      </c>
+      <c r="H2" s="1">
+        <v>650</v>
+      </c>
+      <c r="I2" s="4">
+        <f>G2/(H2/1.081)</f>
+        <v>0.22950461538461539</v>
+      </c>
+      <c r="J2" s="1">
         <v>7</v>
       </c>
+      <c r="K2" s="5">
+        <v>45666</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2020</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1">
+        <v>90</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I6" si="0">G3/(H3/1.081)</f>
+        <v>0.60055555555555551</v>
+      </c>
+      <c r="J3" s="1">
+        <v>12</v>
+      </c>
+      <c r="K3" s="5">
+        <v>45662</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
-        <v>90</v>
-      </c>
-      <c r="F3">
-        <v>12</v>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1">
+        <v>300</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1300</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.24946153846153846</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+      <c r="K4" s="5">
+        <v>45635</v>
+      </c>
+      <c r="L4" s="1">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2020</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1">
+        <v>350</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1450</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26093103448275862</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
+      <c r="K5" s="5">
+        <v>45635</v>
+      </c>
+      <c r="L5" s="1">
+        <v>4</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1">
+        <v>350</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1450</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26093103448275862</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3</v>
+      </c>
+      <c r="K6" s="5">
+        <v>45662</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E4">
-        <v>28</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de la gestion des factures avec lecture des factures via techno OCR
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data.xlsx
+++ b/backend/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\Projets\Stock-V3\backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4928BCD8-447F-4985-81BF-04D2BAF2F14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594DF36F-0A29-4639-988D-3A3F0C9CDD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{866AF031-A8F6-4310-B6CB-F8A451908F4D}"/>
+    <workbookView xWindow="28725" yWindow="-8520" windowWidth="28875" windowHeight="7650" xr2:uid="{866AF031-A8F6-4310-B6CB-F8A451908F4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>Domaine</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>Brut Vintage</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D315F42-56D0-4B9B-B00B-79278325E538}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,6 +783,87 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1">
+        <v>250</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1100</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" ref="I7:I8" si="1">G7/(H7/1.081)</f>
+        <v>0.24568181818181817</v>
+      </c>
+      <c r="J7" s="1">
+        <v>8</v>
+      </c>
+      <c r="K7" s="5">
+        <v>45662</v>
+      </c>
+      <c r="L7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1">
+        <v>38</v>
+      </c>
+      <c r="H8" s="1">
+        <v>130</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31598461538461536</v>
+      </c>
+      <c r="J8" s="1">
+        <v>12</v>
+      </c>
+      <c r="K8" s="5">
+        <v>45662</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Amélioration Design et Structure
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data.xlsx
+++ b/backend/src/main/resources/data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\Projets\Stock-V3\backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594DF36F-0A29-4639-988D-3A3F0C9CDD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C865189-19C2-460D-A6BC-1F80581A0D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28725" yWindow="-8520" windowWidth="28875" windowHeight="7650" xr2:uid="{866AF031-A8F6-4310-B6CB-F8A451908F4D}"/>
+    <workbookView xWindow="2115" yWindow="1065" windowWidth="21600" windowHeight="11385" xr2:uid="{866AF031-A8F6-4310-B6CB-F8A451908F4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Domaine</t>
   </si>
@@ -120,12 +120,58 @@
   </si>
   <si>
     <t>Brut Vintage</t>
+  </si>
+  <si>
+    <t>20Æaine Aligoté Les Jardins de la Cote</t>
+  </si>
+  <si>
+    <t>Domaine Joseph Colin</t>
+  </si>
+  <si>
+    <t>Bourgogne Générique</t>
+  </si>
+  <si>
+    <t>Chardonnay Les Hauts de la Combe</t>
+  </si>
+  <si>
+    <t>Blanc</t>
+  </si>
+  <si>
+    <t>Chassagne-Montrachet</t>
+  </si>
+  <si>
+    <t>En Cailleret</t>
+  </si>
+  <si>
+    <t>Rouge Vieilles Vignes</t>
+  </si>
+  <si>
+    <t>La Garenne</t>
+  </si>
+  <si>
+    <t>Puligny-Montrachet</t>
+  </si>
+  <si>
+    <t>Le Trezin 13</t>
+  </si>
+  <si>
+    <t>Compendium 135</t>
+  </si>
+  <si>
+    <t>Saint-Aubin</t>
+  </si>
+  <si>
+    <t>Clos du Meix 13</t>
+  </si>
+  <si>
+    <t>La Chatenière 135</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -514,22 +560,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D315F42-56D0-4B9B-B00B-79278325E538}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="32.5703125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="19.85546875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" style="1"/>
-    <col min="9" max="9" width="10.140625" style="4" customWidth="1"/>
-    <col min="10" max="12" width="11.42578125" style="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="11.5703125"/>
+    <col min="2" max="3" customWidth="true" style="1" width="32.5703125"/>
+    <col min="4" max="6" customWidth="true" style="1" width="19.85546875"/>
+    <col min="7" max="8" style="1" width="11.42578125"/>
+    <col min="9" max="9" customWidth="true" style="4" width="10.140625"/>
+    <col min="10" max="12" style="1" width="11.42578125"/>
+    <col min="13" max="13" customWidth="true" style="1" width="12.85546875"/>
+    <col min="14" max="16384" style="1" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -864,6 +911,236 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="B9" t="s" s="1">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="G9" t="n" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="J9" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K9" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B10" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="G10" t="n" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="J10" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K10" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B11" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G11" t="n" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="J11" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K11" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B12" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G12" t="n" s="1">
+        <v>78.0</v>
+      </c>
+      <c r="J12" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K12" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B13" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G13" t="n" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="J13" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K13" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B14" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="G14" t="n" s="1">
+        <v>91.0</v>
+      </c>
+      <c r="J14" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K14" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B15" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="G15" t="n" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="J15" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K15" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B16" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G16" t="n" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="J16" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K16" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B17" t="s" s="1">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G17" t="n" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="J17" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K17" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B18" t="s" s="1">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G18" t="n" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="J18" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K18" t="n" s="1">
+        <v>45680.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Css & Html files for more clarity
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data.xlsx
+++ b/backend/src/main/resources/data.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="45">
   <si>
     <t>Domaine</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>La Chatenière 135</t>
+  </si>
+  <si>
+    <t>Domaine Aligoté Les Jardins de la Cote</t>
+  </si>
+  <si>
+    <t>Aligoté Les Jardins de la Cote</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D315F42-56D0-4B9B-B00B-79278325E538}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1141,6 +1147,696 @@
         <v>45680.0</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="B19" t="s" s="1">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="G19" t="n" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="J19" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K19" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B20" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="G20" t="n" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="J20" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K20" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B21" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G21" t="n" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="J21" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K21" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B22" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G22" t="n" s="1">
+        <v>78.0</v>
+      </c>
+      <c r="J22" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K22" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B23" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G23" t="n" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="J23" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K23" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B24" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="G24" t="n" s="1">
+        <v>91.0</v>
+      </c>
+      <c r="J24" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K24" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B25" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="G25" t="n" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="J25" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K25" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B26" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G26" t="n" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="J26" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K26" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B27" t="s" s="1">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G27" t="n" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="J27" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K27" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B28" t="s" s="1">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G28" t="n" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="J28" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K28" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="B29" t="s" s="1">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="G29" t="n" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="J29" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K29" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B30" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="G30" t="n" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="J30" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K30" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B31" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G31" t="n" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="J31" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K31" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B32" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G32" t="n" s="1">
+        <v>78.0</v>
+      </c>
+      <c r="J32" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K32" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B33" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G33" t="n" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="J33" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K33" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B34" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="G34" t="n" s="1">
+        <v>91.0</v>
+      </c>
+      <c r="J34" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K34" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B35" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D35" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="G35" t="n" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="J35" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K35" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B36" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D36" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G36" t="n" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="J36" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K36" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B37" t="s" s="1">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D37" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G37" t="n" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="J37" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K37" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B38" t="s" s="1">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D38" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G38" t="n" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="J38" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K38" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="B39" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D39" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="G39" t="n" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="J39" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K39" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B40" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D40" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="G40" t="n" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="J40" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K40" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B41" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D41" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G41" t="n" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="J41" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K41" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B42" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D42" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G42" t="n" s="1">
+        <v>78.0</v>
+      </c>
+      <c r="J42" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K42" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B43" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C43" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="G43" t="n" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="J43" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K43" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B44" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C44" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="G44" t="n" s="1">
+        <v>91.0</v>
+      </c>
+      <c r="J44" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K44" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B45" t="s" s="1">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D45" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="G45" t="n" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="J45" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K45" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B46" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G46" t="n" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="J46" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K46" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B47" t="s" s="1">
+        <v>41</v>
+      </c>
+      <c r="C47" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D47" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G47" t="n" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="J47" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K47" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n" s="1">
+        <v>2021.0</v>
+      </c>
+      <c r="B48" t="s" s="1">
+        <v>42</v>
+      </c>
+      <c r="C48" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s" s="1">
+        <v>40</v>
+      </c>
+      <c r="G48" t="n" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="J48" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K48" t="n" s="1">
+        <v>45684.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Synchronisation Table Article avec Table Wine
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/data.xlsx
+++ b/backend/src/main/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\Projets\Stock-V3\backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1CA74C-A6AC-46FD-A01C-03B4CFDF30AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E9329D-03CE-4894-BEBF-3304C9D1B871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{866AF031-A8F6-4310-B6CB-F8A451908F4D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
   <si>
     <t>Domaine</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Aligoté Les Jardins de la Cote</t>
+  </si>
+  <si>
+    <t>Full Name</t>
   </si>
 </sst>
 </file>
@@ -559,11 +562,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D315F42-56D0-4B9B-B00B-79278325E538}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,14 +574,15 @@
     <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
     <col min="2" max="3" width="32.5703125" style="1" customWidth="1"/>
     <col min="4" max="6" width="19.85546875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" style="1"/>
-    <col min="9" max="9" width="10.140625" style="4" customWidth="1"/>
-    <col min="10" max="12" width="11.42578125" style="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="98.5703125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="10.140625" style="4" customWidth="1"/>
+    <col min="11" max="13" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="12.85546875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -598,28 +602,31 @@
         <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
@@ -638,28 +645,34 @@
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="1" t="str">
+        <f>CONCATENATE(F2," - ",E2," - ",D2," - ",C2," - ",B2," - ",A2)</f>
+        <v>France - Bourgogne - Gevrey-Chambertin - Geanthet Pansiot - "Vieilles Vignes" - 2018</v>
+      </c>
+      <c r="H2" s="1">
         <v>138</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>650</v>
       </c>
-      <c r="I2" s="4">
-        <f>G2/(H2/1.081)</f>
+      <c r="J2" s="4">
+        <f>H2/(I2/1.081)</f>
         <v>0.22950461538461539</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>7</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="1">
+      <c r="L2" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2020</v>
       </c>
@@ -678,28 +691,34 @@
       <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1" t="str">
+        <f t="shared" ref="G3:G18" si="0">CONCATENATE(F3," - ",E3," - ",D3," - ",C3," - ",B3," - ",A3)</f>
+        <v>France - Bourgogne - Chablis - Patrick Piuze - Terroir Chapelle - 2020</v>
+      </c>
+      <c r="H3" s="1">
         <v>50</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>90</v>
       </c>
-      <c r="I3" s="4">
-        <f t="shared" ref="I3:I6" si="0">G3/(H3/1.081)</f>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J6" si="1">H3/(I3/1.081)</f>
         <v>0.60055555555555551</v>
       </c>
-      <c r="J3" s="1">
-        <v>12</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="1">
+      <c r="K3" s="1">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M3" s="1">
         <v>2</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2010</v>
       </c>
@@ -718,28 +737,34 @@
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Champagne - Champagne - Dom Pérignon - Brut Vintage - Magnum - 2010</v>
+      </c>
+      <c r="H4" s="1">
         <v>300</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>1300</v>
       </c>
-      <c r="I4" s="4">
-        <f t="shared" si="0"/>
+      <c r="J4" s="4">
+        <f t="shared" si="1"/>
         <v>0.24946153846153846</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>3</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="1">
+      <c r="L4" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M4" s="1">
         <v>3</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2009</v>
       </c>
@@ -758,28 +783,34 @@
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Champagne - Champagne - Dom Pérignon - Brut Vintage Rosé - 2009</v>
+      </c>
+      <c r="H5" s="1">
         <v>350</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>1450</v>
       </c>
-      <c r="I5" s="4">
-        <f t="shared" si="0"/>
+      <c r="J5" s="4">
+        <f t="shared" si="1"/>
         <v>0.26093103448275862</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>5</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="1">
+      <c r="L5" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M5" s="1">
         <v>4</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2008</v>
       </c>
@@ -798,28 +829,34 @@
       <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Champagne - Champagne - Dom Pérignon - Brut Vintage Rosé - 2008</v>
+      </c>
+      <c r="H6" s="1">
         <v>350</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>1450</v>
       </c>
-      <c r="I6" s="4">
-        <f t="shared" si="0"/>
+      <c r="J6" s="4">
+        <f t="shared" si="1"/>
         <v>0.26093103448275862</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>3</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="1">
+      <c r="L6" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M6" s="1">
         <v>5</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2005</v>
       </c>
@@ -838,25 +875,31 @@
       <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Champagne - Champagne - Dom Pérignon - Brut Vintage - 2005</v>
+      </c>
+      <c r="H7" s="1">
         <v>250</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>1100</v>
       </c>
-      <c r="I7" s="4">
-        <f t="shared" ref="I7:I8" si="1">G7/(H7/1.081)</f>
+      <c r="J7" s="4">
+        <f t="shared" ref="J7:J8" si="2">H7/(I7/1.081)</f>
         <v>0.24568181818181817</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>8</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="1">
+      <c r="L7" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2021</v>
       </c>
@@ -875,28 +918,34 @@
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Chablis - Patrick Piuze - Terroir Chapelle - 2021</v>
+      </c>
+      <c r="H8" s="1">
         <v>38</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>130</v>
       </c>
-      <c r="I8" s="4">
-        <f t="shared" si="1"/>
+      <c r="J8" s="4">
+        <f t="shared" si="2"/>
         <v>0.31598461538461536</v>
       </c>
-      <c r="J8" s="1">
-        <v>12</v>
-      </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="1">
+      <c r="K8" s="1">
+        <v>12</v>
+      </c>
+      <c r="L8" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M8" s="1">
         <v>7</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2005</v>
       </c>
@@ -915,24 +964,31 @@
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Bourgogne Générique - Domaine Joseph Colin - Aligoté Les Jardins de la Cote - 2005</v>
+      </c>
+      <c r="H9" s="1">
         <v>15</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>130</v>
       </c>
-      <c r="I9" s="4">
-        <f t="shared" ref="I9:I18" si="2">G9/(H9/1.081)</f>
+      <c r="J9" s="4">
+        <f t="shared" ref="J9:J18" si="3">H9/(I9/1.081)</f>
         <v>0.12473076923076923</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>6</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2021</v>
       </c>
@@ -951,24 +1007,31 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Bourgogne Générique - Domaine Joseph Colin - Chardonnay Les Hauts de la Combe - 2021</v>
+      </c>
+      <c r="H10" s="1">
         <v>25</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>130</v>
       </c>
-      <c r="I10" s="4">
-        <f t="shared" si="2"/>
+      <c r="J10" s="4">
+        <f t="shared" si="3"/>
         <v>0.20788461538461539</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>6</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M10" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2021</v>
       </c>
@@ -987,24 +1050,31 @@
       <c r="F11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Chassagne-Montrachet - Domaine Joseph Colin - Blanc - 2021</v>
+      </c>
+      <c r="H11" s="1">
         <v>47</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>130</v>
       </c>
-      <c r="I11" s="4">
-        <f t="shared" si="2"/>
+      <c r="J11" s="4">
+        <f t="shared" si="3"/>
         <v>0.39082307692307694</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>6</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2021</v>
       </c>
@@ -1023,24 +1093,31 @@
       <c r="F12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Chassagne-Montrachet - Domaine Joseph Colin - En Cailleret - 2021</v>
+      </c>
+      <c r="H12" s="1">
         <v>78</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>130</v>
       </c>
-      <c r="I12" s="4">
-        <f t="shared" si="2"/>
+      <c r="J12" s="4">
+        <f t="shared" si="3"/>
         <v>0.64859999999999995</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>6</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M12" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2021</v>
       </c>
@@ -1059,24 +1136,31 @@
       <c r="F13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Chassagne-Montrachet - Domaine Joseph Colin - Rouge Vieilles Vignes - 2021</v>
+      </c>
+      <c r="H13" s="1">
         <v>32</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>130</v>
       </c>
-      <c r="I13" s="4">
-        <f t="shared" si="2"/>
+      <c r="J13" s="4">
+        <f t="shared" si="3"/>
         <v>0.26609230769230768</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>6</v>
       </c>
-      <c r="L13" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2021</v>
       </c>
@@ -1095,24 +1179,31 @@
       <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Puligny-Montrachet - Domaine Joseph Colin - La Garenne - 2021</v>
+      </c>
+      <c r="H14" s="1">
         <v>91</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>130</v>
       </c>
-      <c r="I14" s="4">
-        <f t="shared" si="2"/>
+      <c r="J14" s="4">
+        <f t="shared" si="3"/>
         <v>0.75669999999999993</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>6</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M14" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2021</v>
       </c>
@@ -1131,24 +1222,31 @@
       <c r="F15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Puligny-Montrachet - Domaine Joseph Colin - Le Trezin 13 - 2021</v>
+      </c>
+      <c r="H15" s="1">
         <v>85</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>130</v>
       </c>
-      <c r="I15" s="4">
-        <f t="shared" si="2"/>
+      <c r="J15" s="4">
+        <f t="shared" si="3"/>
         <v>0.70680769230769225</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>6</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M15" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2021</v>
       </c>
@@ -1167,24 +1265,31 @@
       <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Saint-Aubin - Domaine Joseph Colin - Compendium 135 - 2021</v>
+      </c>
+      <c r="H16" s="1">
         <v>32</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>130</v>
       </c>
-      <c r="I16" s="4">
-        <f t="shared" si="2"/>
+      <c r="J16" s="4">
+        <f t="shared" si="3"/>
         <v>0.26609230769230768</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>6</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M16" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2021</v>
       </c>
@@ -1203,24 +1308,31 @@
       <c r="F17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Saint-Aubin - Domaine Joseph Colin - Clos du Meix 13 - 2021</v>
+      </c>
+      <c r="H17" s="1">
         <v>43</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>130</v>
       </c>
-      <c r="I17" s="4">
-        <f t="shared" si="2"/>
+      <c r="J17" s="4">
+        <f t="shared" si="3"/>
         <v>0.35756153846153843</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>6</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M17" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2021</v>
       </c>
@@ -1239,20 +1351,27 @@
       <c r="F18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>France - Bourgogne - Saint-Aubin - Domaine Joseph Colin - La Chatenière 135 - 2021</v>
+      </c>
+      <c r="H18" s="1">
         <v>47</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>130</v>
       </c>
-      <c r="I18" s="4">
-        <f t="shared" si="2"/>
+      <c r="J18" s="4">
+        <f t="shared" si="3"/>
         <v>0.39082307692307694</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <v>6</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="5">
+        <v>45694</v>
+      </c>
+      <c r="M18" s="1">
         <v>17</v>
       </c>
     </row>

</xml_diff>